<commit_message>
Requisito funcional de Gestion de productos con una GUI Jorge Gil
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\nruhhhh\costeoRapido\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7741D6-407A-4ABB-97B5-0C037ADA55C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68830764-C45B-48F9-9335-E7423FFC1A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Productos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -60,12 +60,25 @@
   </si>
   <si>
     <t>Etiquetas</t>
+  </si>
+  <si>
+    <t>Primer producto</t>
+  </si>
+  <si>
+    <t>Camara</t>
+  </si>
+  <si>
+    <t>Ayunagi</t>
+  </si>
+  <si>
+    <t>Saber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -461,9 +474,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="16.0"/>
+    <col min="5" max="5" customWidth="true" width="16.21875"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -492,6 +505,32 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>90.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>675.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -504,15 +543,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F38D122278C567489FDD70CE33BB6DCF" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e56c0d47ec30df08235564da8acf5af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="599d97992d73e44d870b496c783eb150">
     <xsd:element name="properties">
@@ -626,6 +656,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B747568-4481-40AE-8C7E-D4842258D50C}">
   <ds:schemaRefs>
@@ -642,14 +681,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4FC412-43F1-4849-8DB2-F59FD9C8EC36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -663,4 +694,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gestion de productos terminada, solo falta el boton de regresar; JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,48 @@
   </si>
   <si>
     <t>Saber</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Cámara</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>jaf</t>
+  </si>
+  <si>
+    <t>aquaman</t>
+  </si>
+  <si>
+    <t>gay</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>ahaha</t>
+  </si>
+  <si>
+    <t>mynor</t>
+  </si>
+  <si>
+    <t>hipermega gay</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>sdfv</t>
   </si>
 </sst>
 </file>
@@ -466,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -507,28 +549,106 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>750.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>90.0</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>675.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>8.0</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>11</v>
+      <c r="D3" t="n" s="0">
+        <v>7.8</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>7.8</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>780.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aplicación del menú Andre
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\nruhhhh\costeoRapido\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68830764-C45B-48F9-9335-E7423FFC1A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0385AE-59D0-41A7-9F0B-439E6FF0D9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -60,67 +60,12 @@
   </si>
   <si>
     <t>Etiquetas</t>
-  </si>
-  <si>
-    <t>Primer producto</t>
-  </si>
-  <si>
-    <t>Camara</t>
-  </si>
-  <si>
-    <t>Ayunagi</t>
-  </si>
-  <si>
-    <t>Saber</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>Cámara</t>
-  </si>
-  <si>
-    <t>Toledo</t>
-  </si>
-  <si>
-    <t>jaf</t>
-  </si>
-  <si>
-    <t>aquaman</t>
-  </si>
-  <si>
-    <t>gay</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>ahaha</t>
-  </si>
-  <si>
-    <t>mynor</t>
-  </si>
-  <si>
-    <t>hipermega gay</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>hs</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>sdfv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,17 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="16.0"/>
-    <col min="5" max="5" customWidth="true" width="16.21875"/>
-    <col min="6" max="6" customWidth="true" width="14.6640625"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -547,110 +492,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>750.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>15.0</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>7.8</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>7.8</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>780.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -663,6 +504,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F38D122278C567489FDD70CE33BB6DCF" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e56c0d47ec30df08235564da8acf5af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="599d97992d73e44d870b496c783eb150">
     <xsd:element name="properties">
@@ -776,15 +626,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B747568-4481-40AE-8C7E-D4842258D50C}">
   <ds:schemaRefs>
@@ -801,6 +642,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4FC412-43F1-4849-8DB2-F59FD9C8EC36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -814,12 +663,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificaciones de Gestion de productos JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +102,105 @@
   </si>
   <si>
     <t>sfsf</t>
+  </si>
+  <si>
+    <t>sfgs</t>
+  </si>
+  <si>
+    <t>CAMARA</t>
+  </si>
+  <si>
+    <t>saber</t>
+  </si>
+  <si>
+    <t>📷</t>
+  </si>
+  <si>
+    <t>Domo Plástico *CON AUDIO* de 2MP, 20mts IR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cámara PTZ HDCVI Starlight de 2MP y 15x IK10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bala Imou de 3MP (2304 x 1296), Lente de 2.8mm, IR hasta 30m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cámara 4MP de acceso y lectora de placas ANPR, clasificación IP67 e IK10 Dahua Varifocal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMOU GO KIT: 1x IPC-B32P-V2-IMOU imou Cámara Cell Go WiFi , 3MP, IR de 7m ,PIR, Micrófono, Altavoces, Batería Recargable y panel solar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imou Bombillo cámara 5MP WiFi para hogares </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCO DURO DE 1TB, *SEAGATE SKYHAWK* </t>
+  </si>
+  <si>
+    <t>SISTEMA DE ALMACENAMIENTO</t>
+  </si>
+  <si>
+    <t>💾</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCO DURO DE 1TERABYTE B-STOCK </t>
+  </si>
+  <si>
+    <t>TOSHIBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCO DURO DE 4TERABYTES B-STOCK </t>
+  </si>
+  <si>
+    <t>SEAGATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCO DURO DE 8TB, *SEAGATE SKYHAWK* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEAGATE </t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>ACCESORIO CCTV</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>🛒</t>
+  </si>
+  <si>
+    <t>asdfa</t>
+  </si>
+  <si>
+    <t>CONTROL DE ACCESO Y SEGURIDAD</t>
+  </si>
+  <si>
+    <t>gay</t>
+  </si>
+  <si>
+    <t>gaymer</t>
+  </si>
+  <si>
+    <t>🛡</t>
+  </si>
+  <si>
+    <t>SISTEMAS DE RED</t>
+  </si>
+  <si>
+    <t>🌐</t>
+  </si>
+  <si>
+    <t>🔒</t>
+  </si>
+  <si>
+    <t>uD83D\uDD0C</t>
+  </si>
+  <si>
+    <t>🔌</t>
   </si>
 </sst>
 </file>
@@ -496,7 +595,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -540,25 +639,28 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>48.71794871794872</v>
+        <v>25.512820512820515</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>380.0</v>
+        <v>199.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>15.0</v>
+        <v>5.0</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -566,25 +668,28 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>70.38461538461539</v>
+        <v>370.5128205128205</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>549.0</v>
+        <v>2890.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>10.0</v>
+        <v>63.0</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -592,25 +697,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>44.743589743589745</v>
+        <v>78.72</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>349.0</v>
+        <v>614.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>31.0</v>
+        <v>5.0</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -618,25 +726,28 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>51.15384615384615</v>
+        <v>629.4871794871794</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>399.0</v>
+        <v>4910.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -644,25 +755,28 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>115.25641025641026</v>
+        <v>128.07692307692307</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>899.0</v>
+        <v>999.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>18</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -670,25 +784,173 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>300.2564102564103</v>
+        <v>58.84615384615385</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>2342.0</v>
+        <v>459.0</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s" s="0">
         <v>11</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>660.0</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>5148.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>57.69230769230769</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>450.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>142.94871794871796</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>1115.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>332.05128205128204</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>2590.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>115.26</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>899.03</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones de productos JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -201,6 +201,126 @@
   </si>
   <si>
     <t>🔌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco Duro de 10TB, *SEAGATE SKYHAWK DAHUA* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco duro de estado sólido SATA de 2,5 pulgadas para grabado 24/7 de 1 TB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco duro de estado sólido SATA de 2,5 pulgadas para grabado 24/7 de 512 GB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVR De 8 MP/4k de 32 Canales IP, 160 Mbps con 2 Bahías de discos duros de hasta 10 TB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobina de 100 metros de cable UTP Cat 5e CCA, en color blanco anti flama </t>
+  </si>
+  <si>
+    <t>DAHUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobina de Cable UTP Cat6 100% Cobre Anti Flama </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobina de cable *Coaxial RG59*, Sprywire </t>
+  </si>
+  <si>
+    <t>SPRYWIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobina de cable *Exterior con Gel CAT5E* (305mts), SpryWire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobina de cable *Interior CAT6* (305mts), SpryWire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE HDMI DE 15mts 4k 1.4V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE HDMI DE 40mts 1080P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRYWIRE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAX HUB2 4G PANEL DE CONTROL ETHERNET CON SOPORTE PARA LA VERIFICACIÓN FOTOGRÁFICA DE ALARMAS NEGRO </t>
+  </si>
+  <si>
+    <t>AJAX Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAX Hub: Panel de control de seguridad con soporte para la verificación fotográfica de alarmas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAX Systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detector de Metales con contador estadístico de 18 Zonas </t>
+  </si>
+  <si>
+    <t>ZKTECO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energizador para Cerca Eléctrica convencional, YONUSA </t>
+  </si>
+  <si>
+    <t>YONUSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansor de entrada inalámbrica para alarmas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARRERA MARCA ZKTECO DE ALETA BIOMÉTRICA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CERRADURA MARCA ZKTECO PARA PUERTAS DE CRISTAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energizador para Cerca Eléctrica de Alta frecuencia con Interface, YONUSA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router Dahua de doble antena 300 Mbps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AJAX  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router IMOU para cámaras Wi-Fi, encriptado WPS, IPv6  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router inalámbrico N a 300 Mbps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP-LINK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Router inalámbrico AX1800 con tecnología inalámbrica de sexta generación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAHUA Switch PoE Ethernet de 26 Puertos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH 24 PUERTOS POE FE + 1 PUERTO GIGABIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Easy Smart de 8 puertos Gigabit con 4 puertos PoE 8 puertos RJ45 10/100/1000Mbps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch IMOU gigabit duplexor, de 8 puertos, SG108C, RJ45, Puerto MAC, dirección y autoaprendizaje  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch Marca ZKTECO PoE de 24 Puertos 10/100Mbps </t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>as</t>
   </si>
 </sst>
 </file>
@@ -595,7 +715,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -642,10 +762,10 @@
         <v>26</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>25.512820512820515</v>
+        <v>25.51</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>199.0</v>
+        <v>198.978</v>
       </c>
       <c r="E2" t="n" s="0">
         <v>5.0</v>
@@ -654,7 +774,7 @@
         <v>23</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>11</v>
@@ -671,7 +791,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>370.5128205128205</v>
+        <v>370.51</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>2890.0</v>
@@ -683,7 +803,7 @@
         <v>23</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>11</v>
@@ -729,7 +849,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>629.4871794871794</v>
+        <v>629.49</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>4910.0</v>
@@ -741,7 +861,7 @@
         <v>23</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s" s="0">
         <v>11</v>
@@ -828,7 +948,7 @@
         <v>33</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>11</v>
@@ -926,16 +1046,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>115.26</v>
+        <v>482.43589743589746</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>899.03</v>
+        <v>3763.0</v>
       </c>
       <c r="E12" t="n" s="0">
         <v>3.0</v>
@@ -944,12 +1064,824 @@
         <v>33</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>80.77</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>630.01</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>56.92</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>443.98</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>287.82</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>2245.0</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>19.23</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>51.0</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>141.02564102564102</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>1100.0</v>
+      </c>
+      <c r="E17" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>63.97</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>499.0</v>
+      </c>
+      <c r="E18" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>83.97</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>654.966</v>
+      </c>
+      <c r="E19" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="H19" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>67.82051282051282</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>529.0</v>
+      </c>
+      <c r="E20" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="H20" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>25.512820512820515</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>199.0</v>
+      </c>
+      <c r="E21" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>91.03</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>710.0</v>
+      </c>
+      <c r="E22" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>384.62</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>3000.0</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>1802.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>14055.6</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="H24" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>1139.6153846153845</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>8889.0</v>
+      </c>
+      <c r="E25" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>272.5641025641026</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>2126.0</v>
+      </c>
+      <c r="E26" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="H26" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>29.74</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>231.97199999999998</v>
+      </c>
+      <c r="E27" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H27" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>3307.6923076923076</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>25800.0</v>
+      </c>
+      <c r="E28" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>203.71794871794873</v>
+      </c>
+      <c r="D29" t="n" s="0">
+        <v>1589.0</v>
+      </c>
+      <c r="E29" t="n" s="0">
+        <v>69.0</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I29" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>341.4102564102564</v>
+      </c>
+      <c r="D30" t="n" s="0">
+        <v>2663.0</v>
+      </c>
+      <c r="E30" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I30" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>22.94871794871795</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>179.0</v>
+      </c>
+      <c r="E31" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C32" t="n" s="0">
+        <v>17.307692307692307</v>
+      </c>
+      <c r="D32" t="n" s="0">
+        <v>135.0</v>
+      </c>
+      <c r="E32" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F32" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>19.871794871794872</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>155.0</v>
+      </c>
+      <c r="E33" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F33" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="H33" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>84.48717948717949</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>659.0</v>
+      </c>
+      <c r="E34" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F34" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>284.87179487179486</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>2222.0</v>
+      </c>
+      <c r="E35" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F35" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H35" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I35" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>217.95</v>
+      </c>
+      <c r="D36" t="n" s="0">
+        <v>1700.0</v>
+      </c>
+      <c r="E36" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F36" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="H36" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>63.46153846153846</v>
+      </c>
+      <c r="D37" t="n" s="0">
+        <v>495.0</v>
+      </c>
+      <c r="E37" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F37" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="H37" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I37" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C38" t="n" s="0">
+        <v>26.41</v>
+      </c>
+      <c r="D38" t="n" s="0">
+        <v>206.0</v>
+      </c>
+      <c r="E38" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F38" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H38" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>179.35897435897436</v>
+      </c>
+      <c r="D39" t="n" s="0">
+        <v>1399.0</v>
+      </c>
+      <c r="E39" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="F39" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="H39" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>1.2820512820512822</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="H40" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s" s="0">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalización de Algoritmos para los productos similares JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mynit\OneDrive\Escritorio\POO\costeoRapido\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\nruhhhh\costeoRapido\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D7B69-EC61-445D-8BF5-830E30679B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3873AE5-3AE6-4252-BAA0-21B38FE65625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
+    <workbookView xWindow="2556" yWindow="636" windowWidth="17280" windowHeight="8880" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -246,12 +246,31 @@
   </si>
   <si>
     <t>as</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -306,14 +325,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,17 +682,17 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="16.0"/>
+    <col min="5" max="5" customWidth="true" width="16.33203125"/>
+    <col min="6" max="6" customWidth="true" width="14.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,1020 +717,1026 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="I1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>25.51</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>198.97800000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>370.51</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>2890</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>63</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>78.72</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>614</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>629.49</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>4910</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>128.07692309999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>999</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>58.84615385</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>459</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>660</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>5148</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>57.69230769</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>450</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>142.94871789999999</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>1115</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="0">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>332.05128209999998</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>2590</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0">
         <v>6</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="0">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>482.43589739999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>3763</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="0">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0">
         <v>80.77</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0">
         <v>630.01</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="0">
         <v>2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="0">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>56.92</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <v>443.98</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="0">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="0">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="0">
         <v>287.82</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0">
         <v>2245</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="0">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>19.23</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0">
         <v>150</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="0">
         <v>51</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="0">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0">
         <v>141.02564100000001</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0">
         <v>1100</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="0">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="0">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="0">
         <v>63.97</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0">
         <v>499</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="0">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="0">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="0">
         <v>83.97</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0">
         <v>654.96600000000001</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="0">
         <v>8</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="0">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="0">
         <v>67.820512820000005</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0">
         <v>529</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="0">
         <v>9</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="0">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="0">
         <v>25.512820510000001</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0">
         <v>199</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="0">
         <v>8</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="0">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="0">
         <v>91.03</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0">
         <v>710</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="0">
         <v>5</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" t="s" s="0">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="0">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="0">
         <v>384.62</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0">
         <v>3000</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="0">
         <v>5</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="0">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="0">
         <v>1802</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="0">
         <v>14055.6</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="0">
         <v>9</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="0">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="0">
         <v>1139.6153850000001</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="0">
         <v>8889</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="0">
         <v>7</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="0">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="0">
         <v>272.56410260000001</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="0">
         <v>2126</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="0">
         <v>6</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" t="s" s="0">
         <v>30</v>
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="0">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
         <v>29.74</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="0">
         <v>231.97200000000001</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="0">
         <v>4</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="0">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="0">
         <v>3307.6923080000001</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="0">
         <v>25800</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="0">
         <v>6</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="0">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="0">
         <v>203.71794869999999</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="0">
         <v>1589</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="0">
         <v>69</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="0">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="0">
         <v>341.41025639999998</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="0">
         <v>2663</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="0">
         <v>9</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="0">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="0">
         <v>22.948717949999999</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="0">
         <v>179</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="0">
         <v>8</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="0">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="0">
         <v>17.30769231</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="0">
         <v>135</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="0">
         <v>5</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="0">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="0">
         <v>19.871794869999999</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="0">
         <v>155</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="0">
         <v>9</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="0">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="0">
         <v>84.487179490000003</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="0">
         <v>659</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="0">
         <v>9</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="0">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="0">
         <v>284.8717949</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="0">
         <v>2222</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="0">
         <v>9</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="0">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="0">
         <v>217.95</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="0">
         <v>1700</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="0">
         <v>8</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="0">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="0">
         <v>63.46153846</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="0">
         <v>495</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="0">
         <v>9</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="0">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="0">
         <v>26.41</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="0">
         <v>206</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="0">
         <v>2</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="0">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="0">
         <v>179.35897439999999</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="0">
         <v>1399</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="0">
         <v>9</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40">
-        <v>1.2820512820000001</v>
-      </c>
-      <c r="D40">
-        <v>10</v>
-      </c>
-      <c r="E40">
-        <v>8</v>
-      </c>
-      <c r="F40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" t="s">
-        <v>69</v>
-      </c>
-      <c r="I40" t="s">
-        <v>19</v>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>0.77</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>6.01</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="H40" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1714,6 +1751,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F38D122278C567489FDD70CE33BB6DCF" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e56c0d47ec30df08235564da8acf5af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="599d97992d73e44d870b496c783eb150">
     <xsd:element name="properties">
@@ -1827,15 +1873,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B747568-4481-40AE-8C7E-D4842258D50C}">
   <ds:schemaRefs>
@@ -1852,6 +1889,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4FC412-43F1-4849-8DB2-F59FD9C8EC36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1865,12 +1910,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
arreglar la GUI principal + productos similares + algoritmo de productos similares + menu JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Documents\nruhhhh\costeoRapido\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3873AE5-3AE6-4252-BAA0-21B38FE65625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C903EB-F4EF-4E7D-9988-AA646E35CDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2556" yWindow="636" windowWidth="17280" windowHeight="8880" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
+    <workbookView xWindow="6048" yWindow="852" windowWidth="17280" windowHeight="8880" xr2:uid="{F0218E9C-B69B-4AFC-8A07-E6291C227E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -242,12 +242,6 @@
     <t xml:space="preserve">Switch Marca ZKTECO PoE de 24 Puertos 10/100Mbps </t>
   </si>
   <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
     <t>Otros</t>
   </si>
   <si>
@@ -260,10 +254,25 @@
     <t>w</t>
   </si>
   <si>
-    <t>sd</t>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>alcatel</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>gay DE RED</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>gay</t>
+  </si>
+  <si>
+    <t>mierda</t>
   </si>
 </sst>
 </file>
@@ -302,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -325,26 +334,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,8 +714,8 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>70</v>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1708,35 +1705,6 @@
       </c>
       <c r="I39" t="s" s="0">
         <v>29</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n" s="0">
-        <v>40.0</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C40" t="n" s="0">
-        <v>0.77</v>
-      </c>
-      <c r="D40" t="n" s="0">
-        <v>6.01</v>
-      </c>
-      <c r="E40" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="F40" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G40" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H40" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="I40" t="s" s="0">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1751,15 +1719,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F38D122278C567489FDD70CE33BB6DCF" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e56c0d47ec30df08235564da8acf5af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="599d97992d73e44d870b496c783eb150">
     <xsd:element name="properties">
@@ -1873,6 +1832,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B747568-4481-40AE-8C7E-D4842258D50C}">
   <ds:schemaRefs>
@@ -1889,14 +1857,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F4FC412-43F1-4849-8DB2-F59FD9C8EC36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1910,4 +1870,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024D7F2C-AA19-4C9B-8D3C-EC3758B4253B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
arreglo de problemas en gesiton productos JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -273,6 +273,21 @@
   </si>
   <si>
     <t>mierda</t>
+  </si>
+  <si>
+    <t>asfaa</t>
+  </si>
+  <si>
+    <t>afaf</t>
+  </si>
+  <si>
+    <t>adasd</t>
+  </si>
+  <si>
+    <t>sfsf</t>
+  </si>
+  <si>
+    <t>gay DE ACCESO Y SEGURIDAD</t>
   </si>
 </sst>
 </file>
@@ -676,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1688,14 +1703,14 @@
       <c r="B39" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="C39" s="0">
-        <v>179.35897439999999</v>
-      </c>
-      <c r="D39" s="0">
-        <v>1399</v>
-      </c>
-      <c r="E39" s="0">
-        <v>9</v>
+      <c r="C39" s="0" t="n">
+        <v>179.35897435897436</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>1399.0</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>9.0</v>
       </c>
       <c r="F39" t="s" s="0">
         <v>28</v>
@@ -1703,8 +1718,40 @@
       <c r="G39" t="s" s="0">
         <v>51</v>
       </c>
+      <c r="H39" t="s" s="0">
+        <v>76</v>
+      </c>
       <c r="I39" t="s" s="0">
         <v>29</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>1560.0</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>65.0</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="H40" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="I40" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diseño de interfaces JAGL
</commit_message>
<xml_diff>
--- a/resources/productos.xlsx
+++ b/resources/productos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -691,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE51EEC-3CB5-43EB-96F5-8B3C8F4A3126}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -766,20 +766,23 @@
       <c r="B3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3" s="0" t="n">
         <v>370.51</v>
       </c>
-      <c r="D3" s="0">
-        <v>2890</v>
-      </c>
-      <c r="E3" s="0">
-        <v>63</v>
+      <c r="D3" s="0" t="n">
+        <v>2890.0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>63.0</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>32</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>76</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>10</v>
@@ -1723,35 +1726,6 @@
       </c>
       <c r="I39" t="s" s="0">
         <v>29</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n" s="0">
-        <v>40.0</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="C40" t="n" s="0">
-        <v>1.2820512820512822</v>
-      </c>
-      <c r="D40" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="E40" t="n" s="0">
-        <v>65.0</v>
-      </c>
-      <c r="F40" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="G40" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H40" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="I40" t="s" s="0">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>